<commit_message>
Complete set of insights app and newsblogxml
</commit_message>
<xml_diff>
--- a/data/InsightApp_TC01.xlsx
+++ b/data/InsightApp_TC01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>TestYourInsightAppURL</t>
   </si>
@@ -72,9 +72,6 @@
     <t>ContactUSComp</t>
   </si>
   <si>
-    <t>compSel</t>
-  </si>
-  <si>
     <t>Tyou</t>
   </si>
   <si>
@@ -82,6 +79,21 @@
   </si>
   <si>
     <t>10002</t>
+  </si>
+  <si>
+    <t>NegZipCode1</t>
+  </si>
+  <si>
+    <t>NegZipCode2</t>
+  </si>
+  <si>
+    <t>PosZipCode</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>1$#abcd234</t>
   </si>
 </sst>
 </file>
@@ -159,7 +171,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -169,6 +181,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,10 +535,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -533,14 +546,14 @@
     <col min="1" max="1" width="21.140625"/>
     <col min="2" max="3" width="11.5703125"/>
     <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="10.140625"/>
-    <col min="6" max="6" width="9.42578125"/>
-    <col min="7" max="7" width="11.5703125"/>
-    <col min="8" max="8" width="8.28515625"/>
-    <col min="9" max="985" width="11.5703125"/>
+    <col min="8" max="8" width="10.140625"/>
+    <col min="9" max="9" width="9.42578125"/>
+    <col min="10" max="10" width="11.5703125"/>
+    <col min="11" max="11" width="8.28515625"/>
+    <col min="12" max="987" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,29 +566,35 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -586,34 +605,40 @@
         <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>19</v>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location="/insights"/>
-    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId3"/>

</xml_diff>